<commit_message>
write chosing row in dataGridView
</commit_message>
<xml_diff>
--- a/WindowsFormsApp1/bin/Debug/RussianCity.xlsx
+++ b/WindowsFormsApp1/bin/Debug/RussianCity.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Код города</t>
   </si>
@@ -27,31 +27,16 @@
     <t>Регион</t>
   </si>
   <si>
-    <t>Казань</t>
+    <t>Новосибирск</t>
+  </si>
+  <si>
+    <t>Новосибирская область</t>
+  </si>
+  <si>
+    <t>Набережные Челны</t>
   </si>
   <si>
     <t>Татарстан</t>
-  </si>
-  <si>
-    <t>Новосибирск</t>
-  </si>
-  <si>
-    <t>Новосибирская область</t>
-  </si>
-  <si>
-    <t>Ульяновск</t>
-  </si>
-  <si>
-    <t>Ульяновская область</t>
-  </si>
-  <si>
-    <t>Набережные Челны</t>
-  </si>
-  <si>
-    <t>Уфа</t>
-  </si>
-  <si>
-    <t>Башкортостан</t>
   </si>
 </sst>
 </file>
@@ -391,13 +376,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,74 +400,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>8843</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>383</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>383</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>88552</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>8422</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>88552</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>8347</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>